<commit_message>
finish the create player dna system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/PlayerDna.xlsx
+++ b/ConfigData/Xlsx/PlayerDna.xlsx
@@ -18,8 +18,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>张剑慧</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>张剑慧:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+1.左
+2.右
+3.两边</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -50,10 +88,6 @@
     <t>Url</t>
   </si>
   <si>
-    <t>tmp</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>互斥组</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -90,10 +124,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>缓</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>仁</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -101,42 +131,6 @@
     <t>灭</t>
   </si>
   <si>
-    <t>忠</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>奸</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>动</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>静</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>清</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>浊</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>灰</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>白</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>黑</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>14,15</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -210,6 +204,257 @@
   </si>
   <si>
     <t>金</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>连接类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LineType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ice</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fire</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>slow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fast</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ghost</t>
+  </si>
+  <si>
+    <t>kill</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ba</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>xu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hun</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sky</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>弓</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>剑</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sword</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>叶</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>果</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ye</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>guo</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kong</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yuan</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>reng</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tan</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>nu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>贪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jiao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>round</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>方</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>角</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圆</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>思</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>热情，执着，猛烈</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷静，冷库，沉着</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>迅捷如风，迅雷不及</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>机智，智者千虑</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>仁德，包容世界</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>横扫千军如卷席</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>贪得无厌，得一望十</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>嗔目切齿，睚眦必报</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>左右开弓，百步穿杨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>刀光剑影，一剑封喉</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>掌控时间，来去自如</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>空间转换，若有若无</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>原始自然，万物归一</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>秩序，律法，统一</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>混沌，自由，野性</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>青山绿水万物新</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>万紫千红总是春</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>规则，棱角</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>尖锐，突进</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>和谐，统一</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>天人归一，物竞天择</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>亡者之书，异灵之力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>【高难度】天下虽大，唯我独尊</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>【高难度】有钱能使鬼推磨</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -217,7 +462,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +657,21 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -975,76 +1235,23 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="26">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1060,17 +1267,48 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <family val="2"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1105,6 +1343,8 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -1218,6 +1458,111 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1300,17 +1645,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:E27" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A3:E27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H27" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="A3:H27"/>
   <sortState ref="A4:D4">
     <sortCondition ref="A3:A4"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Id" dataDxfId="15"/>
-    <tableColumn id="2" name="Name" dataDxfId="14"/>
-    <tableColumn id="5" name="Des" dataDxfId="10"/>
-    <tableColumn id="4" name="MutexId" dataDxfId="12"/>
-    <tableColumn id="3" name="Url" dataDxfId="13"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Id" dataDxfId="7"/>
+    <tableColumn id="2" name="Name" dataDxfId="6"/>
+    <tableColumn id="5" name="Des" dataDxfId="5"/>
+    <tableColumn id="4" name="MutexId" dataDxfId="4"/>
+    <tableColumn id="6" name="X" dataDxfId="3"/>
+    <tableColumn id="7" name="Y" dataDxfId="2"/>
+    <tableColumn id="8" name="LineType" dataDxfId="1"/>
+    <tableColumn id="3" name="Url" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1636,27 +1984,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="7.375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="7.375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.25" style="4" customWidth="1"/>
     <col min="3" max="3" width="24.625" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="9" style="4"/>
-    <col min="7" max="7" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="4"/>
+    <col min="5" max="6" width="4.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6" style="4" customWidth="1"/>
+    <col min="8" max="9" width="9" style="4"/>
+    <col min="10" max="10" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1664,16 +2015,25 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1681,16 +2041,25 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -1698,427 +2067,722 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="D4" s="10">
         <v>2</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>8</v>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10">
+        <v>2</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>2</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="D5" s="10">
         <v>1</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>8</v>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10">
+        <v>1</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="D6" s="10">
         <v>4</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>8</v>
+      <c r="E6" s="10">
+        <v>2</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>2</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>4</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="10"/>
+        <v>76</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="D7" s="10">
         <v>3</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>8</v>
+      <c r="E7" s="10">
+        <v>3</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>5</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="D8" s="10">
         <v>6</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>8</v>
+      <c r="E8" s="10">
+        <v>4</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>2</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>6</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="10"/>
+        <v>18</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="D9" s="10">
         <v>5</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>8</v>
+      <c r="E9" s="10">
+        <v>5</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="10"/>
+        <v>68</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="D10" s="10">
         <v>8</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>8</v>
+      <c r="E10" s="10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="10">
+        <v>2</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <v>8</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="10"/>
+        <v>69</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>84</v>
+      </c>
       <c r="D11" s="10">
         <v>7</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>8</v>
+      <c r="E11" s="10">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <v>9</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="10"/>
+        <v>54</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="D12" s="10">
         <v>10</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>8</v>
+      <c r="E12" s="10">
+        <v>2</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <v>10</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="10"/>
+        <v>55</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="D13" s="10">
         <v>9</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>8</v>
+      <c r="E13" s="10">
+        <v>3</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" s="10">
+        <v>1</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="10"/>
+        <v>58</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="D14" s="10">
         <v>12</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>8</v>
+      <c r="E14" s="10">
+        <v>4</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+      <c r="G14" s="10">
+        <v>2</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <v>12</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="10"/>
+        <v>59</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="D15" s="10">
         <v>11</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>8</v>
+      <c r="E15" s="10">
+        <v>5</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1</v>
+      </c>
+      <c r="G15" s="10">
+        <v>1</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="9">
         <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="10"/>
+        <v>73</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>94</v>
+      </c>
       <c r="D16" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0</v>
+      </c>
+      <c r="F16" s="10">
+        <v>2</v>
+      </c>
+      <c r="G16" s="10">
+        <v>2</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="9">
         <v>14</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="10"/>
+        <v>74</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>95</v>
+      </c>
       <c r="D17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>8</v>
+        <v>21</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1</v>
+      </c>
+      <c r="F17" s="10">
+        <v>2</v>
+      </c>
+      <c r="G17" s="10">
+        <v>3</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="9">
         <v>15</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="10"/>
+        <v>75</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="D18" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="E18" s="10">
+        <v>2</v>
+      </c>
+      <c r="F18" s="10">
+        <v>2</v>
+      </c>
+      <c r="G18" s="10">
+        <v>1</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="9">
         <v>16</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="D19" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="E19" s="10">
+        <v>3</v>
+      </c>
+      <c r="F19" s="10">
+        <v>2</v>
+      </c>
+      <c r="G19" s="10">
+        <v>2</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="9">
         <v>17</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>88</v>
+      </c>
       <c r="D20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="E20" s="11">
+        <v>4</v>
+      </c>
+      <c r="F20" s="11">
+        <v>2</v>
+      </c>
+      <c r="G20" s="10">
+        <v>3</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="9">
         <v>18</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="D21" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>8</v>
+        <v>27</v>
+      </c>
+      <c r="E21" s="11">
+        <v>5</v>
+      </c>
+      <c r="F21" s="11">
+        <v>2</v>
+      </c>
+      <c r="G21" s="10">
+        <v>1</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="9">
         <v>19</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="10"/>
+        <v>28</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="D22" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>8</v>
+        <v>32</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0</v>
+      </c>
+      <c r="F22" s="11">
+        <v>3</v>
+      </c>
+      <c r="G22" s="11">
+        <v>2</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="9">
         <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="D23" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="E23" s="10">
+        <v>1</v>
+      </c>
+      <c r="F23" s="11">
+        <v>3</v>
+      </c>
+      <c r="G23" s="11">
+        <v>3</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="9">
         <v>21</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="10"/>
+        <v>31</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>97</v>
+      </c>
       <c r="D24" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>8</v>
+        <v>34</v>
+      </c>
+      <c r="E24" s="10">
+        <v>2</v>
+      </c>
+      <c r="F24" s="11">
+        <v>3</v>
+      </c>
+      <c r="G24" s="11">
+        <v>3</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" s="9">
         <v>22</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>98</v>
+      </c>
       <c r="D25" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>8</v>
+        <v>35</v>
+      </c>
+      <c r="E25" s="10">
+        <v>3</v>
+      </c>
+      <c r="F25" s="11">
+        <v>3</v>
+      </c>
+      <c r="G25" s="11">
+        <v>1</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="9">
         <v>23</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="10"/>
+        <v>36</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>99</v>
+      </c>
       <c r="D26" s="11"/>
-      <c r="E26" s="11" t="s">
-        <v>8</v>
+      <c r="E26" s="11">
+        <v>4</v>
+      </c>
+      <c r="F26" s="11">
+        <v>3</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="9">
         <v>24</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="10"/>
+        <v>37</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>100</v>
+      </c>
       <c r="D27" s="11"/>
-      <c r="E27" s="11" t="s">
-        <v>8</v>
+      <c r="E27" s="11">
+        <v>5</v>
+      </c>
+      <c r="F27" s="11">
+        <v>3</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:E13">
-    <cfRule type="containsBlanks" dxfId="11" priority="10">
+  <conditionalFormatting sqref="B6:F9 B10:D13 F10:F15 B4:H5 H6:H13">
+    <cfRule type="containsBlanks" dxfId="25" priority="15">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:E15">
-    <cfRule type="containsBlanks" dxfId="8" priority="9">
+  <conditionalFormatting sqref="B14:D15 H14:H15 F14:F15">
+    <cfRule type="containsBlanks" dxfId="24" priority="14">
       <formula>LEN(TRIM(B14))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:E17">
-    <cfRule type="containsBlanks" dxfId="7" priority="8">
+  <conditionalFormatting sqref="B16:H17">
+    <cfRule type="containsBlanks" dxfId="23" priority="13">
       <formula>LEN(TRIM(B16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+    <cfRule type="containsBlanks" dxfId="22" priority="12">
       <formula>LEN(TRIM(C18))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(E18))=0</formula>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="containsBlanks" dxfId="21" priority="11">
+      <formula>LEN(TRIM(H18))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:E20">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+  <conditionalFormatting sqref="B19:F20 H19:H20">
+    <cfRule type="containsBlanks" dxfId="20" priority="10">
       <formula>LEN(TRIM(B19))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="19" priority="9">
       <formula>LEN(TRIM(C21))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(E21))=0</formula>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="containsBlanks" dxfId="18" priority="8">
+      <formula>LEN(TRIM(H21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="17" priority="7">
       <formula>LEN(TRIM(C22))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E27">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+  <conditionalFormatting sqref="H22:H27">
+    <cfRule type="containsBlanks" dxfId="16" priority="6">
+      <formula>LEN(TRIM(H22))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6:G15">
+    <cfRule type="containsBlanks" dxfId="15" priority="5">
+      <formula>LEN(TRIM(G6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E15">
+    <cfRule type="containsBlanks" dxfId="14" priority="4">
+      <formula>LEN(TRIM(E10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19:G20">
+    <cfRule type="containsBlanks" dxfId="13" priority="3">
+      <formula>LEN(TRIM(G19))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:E23">
+    <cfRule type="containsBlanks" dxfId="12" priority="2">
       <formula>LEN(TRIM(E22))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E26">
+    <cfRule type="containsBlanks" dxfId="11" priority="1">
+      <formula>LEN(TRIM(E25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change some dna icon
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/PlayerDna.xlsx
+++ b/ConfigData/Xlsx/PlayerDna.xlsx
@@ -199,14 +199,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>霸</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>金</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>X</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -250,10 +242,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>gold</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ba</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -454,7 +442,18 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>【高难度】有钱能使鬼推磨</t>
+    <t>泓</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>煌</t>
+  </si>
+  <si>
+    <t>【高难度】一泓清水明月照</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hong</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1988,10 +1987,10 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2021,13 +2020,13 @@
         <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -2047,13 +2046,13 @@
         <v>9</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>1</v>
@@ -2073,13 +2072,13 @@
         <v>10</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>7</v>
@@ -2093,7 +2092,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D4" s="10">
         <v>2</v>
@@ -2108,7 +2107,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -2119,7 +2118,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D5" s="10">
         <v>1</v>
@@ -2134,7 +2133,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
@@ -2145,7 +2144,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D6" s="10">
         <v>4</v>
@@ -2160,7 +2159,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
@@ -2168,10 +2167,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D7" s="10">
         <v>3</v>
@@ -2186,7 +2185,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
@@ -2197,7 +2196,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D8" s="10">
         <v>6</v>
@@ -2212,7 +2211,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
@@ -2223,7 +2222,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D9" s="10">
         <v>5</v>
@@ -2238,7 +2237,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
@@ -2246,10 +2245,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D10" s="10">
         <v>8</v>
@@ -2264,7 +2263,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
@@ -2272,10 +2271,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D11" s="10">
         <v>7</v>
@@ -2290,7 +2289,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
@@ -2298,10 +2297,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D12" s="10">
         <v>10</v>
@@ -2316,7 +2315,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
@@ -2324,10 +2323,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D13" s="10">
         <v>9</v>
@@ -2342,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
@@ -2350,10 +2349,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D14" s="10">
         <v>12</v>
@@ -2368,7 +2367,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
@@ -2376,10 +2375,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D15" s="10">
         <v>11</v>
@@ -2394,7 +2393,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
@@ -2402,10 +2401,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>19</v>
@@ -2420,7 +2419,7 @@
         <v>2</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
@@ -2428,10 +2427,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>21</v>
@@ -2446,7 +2445,7 @@
         <v>3</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
@@ -2454,10 +2453,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>20</v>
@@ -2472,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
@@ -2483,7 +2482,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>25</v>
@@ -2498,7 +2497,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
@@ -2509,7 +2508,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>26</v>
@@ -2524,7 +2523,7 @@
         <v>3</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
@@ -2535,7 +2534,7 @@
         <v>24</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>27</v>
@@ -2550,7 +2549,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
@@ -2561,7 +2560,7 @@
         <v>28</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>32</v>
@@ -2576,7 +2575,7 @@
         <v>2</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
@@ -2587,7 +2586,7 @@
         <v>29</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>33</v>
@@ -2602,7 +2601,7 @@
         <v>3</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
@@ -2613,7 +2612,7 @@
         <v>31</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>34</v>
@@ -2628,7 +2627,7 @@
         <v>3</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
@@ -2639,7 +2638,7 @@
         <v>30</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>35</v>
@@ -2654,7 +2653,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
@@ -2662,10 +2661,10 @@
         <v>23</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11">
@@ -2676,7 +2675,7 @@
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
@@ -2684,10 +2683,10 @@
         <v>24</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="11">
@@ -2698,7 +2697,7 @@
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rearrage the dna lelated code
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/PlayerDna.xlsx
+++ b/ConfigData/Xlsx/PlayerDna.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="104">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -454,6 +454,18 @@
   </si>
   <si>
     <t>hong</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>~Calculater</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -672,7 +684,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -867,6 +879,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1146,7 +1164,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1187,6 +1205,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1234,7 +1258,33 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1270,6 +1320,111 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1457,111 +1612,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1644,20 +1694,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H27" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="A3:H27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:I27" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" tableBorderDxfId="24">
+  <autoFilter ref="A3:I27"/>
   <sortState ref="A4:D4">
     <sortCondition ref="A3:A4"/>
   </sortState>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Id" dataDxfId="7"/>
-    <tableColumn id="2" name="Name" dataDxfId="6"/>
-    <tableColumn id="5" name="Des" dataDxfId="5"/>
-    <tableColumn id="4" name="MutexId" dataDxfId="4"/>
-    <tableColumn id="6" name="X" dataDxfId="3"/>
-    <tableColumn id="7" name="Y" dataDxfId="2"/>
-    <tableColumn id="8" name="LineType" dataDxfId="1"/>
-    <tableColumn id="3" name="Url" dataDxfId="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Id" dataDxfId="23"/>
+    <tableColumn id="2" name="Name" dataDxfId="22"/>
+    <tableColumn id="5" name="Des" dataDxfId="21"/>
+    <tableColumn id="4" name="MutexId" dataDxfId="20"/>
+    <tableColumn id="6" name="X" dataDxfId="19"/>
+    <tableColumn id="7" name="Y" dataDxfId="18"/>
+    <tableColumn id="8" name="LineType" dataDxfId="2"/>
+    <tableColumn id="9" name="~Calculater" dataDxfId="0">
+      <calculatedColumnFormula>POWER(2,A4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Url" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1984,13 +2037,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2001,12 +2054,13 @@
     <col min="4" max="4" width="12.625" style="4" customWidth="1"/>
     <col min="5" max="6" width="4.5" style="4" customWidth="1"/>
     <col min="7" max="7" width="6" style="4" customWidth="1"/>
-    <col min="8" max="9" width="9" style="4"/>
-    <col min="10" max="10" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="4"/>
+    <col min="8" max="8" width="9.75" style="4" customWidth="1"/>
+    <col min="9" max="10" width="9" style="4"/>
+    <col min="11" max="11" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2028,11 +2082,14 @@
       <c r="G1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2054,11 +2111,14 @@
       <c r="G2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -2081,10 +2141,13 @@
         <v>40</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2106,11 +2169,15 @@
       <c r="G4" s="10">
         <v>2</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="14">
+        <f t="shared" ref="H4:H27" si="0">POWER(2,A4)</f>
+        <v>2</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2132,11 +2199,15 @@
       <c r="G5" s="10">
         <v>1</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2158,11 +2229,15 @@
       <c r="G6" s="10">
         <v>2</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2184,11 +2259,15 @@
       <c r="G7" s="10">
         <v>1</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="14">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2210,11 +2289,15 @@
       <c r="G8" s="10">
         <v>2</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="14">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2236,11 +2319,15 @@
       <c r="G9" s="10">
         <v>1</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="14">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -2262,11 +2349,15 @@
       <c r="G10" s="10">
         <v>2</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="14">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2288,11 +2379,15 @@
       <c r="G11" s="10">
         <v>1</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="14">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2314,11 +2409,15 @@
       <c r="G12" s="10">
         <v>2</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="14">
+        <f t="shared" si="0"/>
+        <v>512</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2340,11 +2439,15 @@
       <c r="G13" s="10">
         <v>1</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="14">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+      <c r="I13" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -2366,11 +2469,15 @@
       <c r="G14" s="10">
         <v>2</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="14">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="I14" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -2392,11 +2499,15 @@
       <c r="G15" s="10">
         <v>1</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="14">
+        <f t="shared" si="0"/>
+        <v>4096</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -2418,11 +2529,15 @@
       <c r="G16" s="10">
         <v>2</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="14">
+        <f t="shared" si="0"/>
+        <v>8192</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -2444,11 +2559,15 @@
       <c r="G17" s="10">
         <v>3</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="14">
+        <f t="shared" si="0"/>
+        <v>16384</v>
+      </c>
+      <c r="I17" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -2470,11 +2589,15 @@
       <c r="G18" s="10">
         <v>1</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="14">
+        <f t="shared" si="0"/>
+        <v>32768</v>
+      </c>
+      <c r="I18" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -2496,11 +2619,15 @@
       <c r="G19" s="10">
         <v>2</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="14">
+        <f t="shared" si="0"/>
+        <v>65536</v>
+      </c>
+      <c r="I19" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -2522,11 +2649,15 @@
       <c r="G20" s="10">
         <v>3</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="14">
+        <f t="shared" si="0"/>
+        <v>131072</v>
+      </c>
+      <c r="I20" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -2548,11 +2679,15 @@
       <c r="G21" s="10">
         <v>1</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="14">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -2574,11 +2709,15 @@
       <c r="G22" s="11">
         <v>2</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="15">
+        <f t="shared" si="0"/>
+        <v>524288</v>
+      </c>
+      <c r="I22" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -2600,11 +2739,15 @@
       <c r="G23" s="11">
         <v>3</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="15">
+        <f t="shared" si="0"/>
+        <v>1048576</v>
+      </c>
+      <c r="I23" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -2626,11 +2769,15 @@
       <c r="G24" s="11">
         <v>3</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="15">
+        <f t="shared" si="0"/>
+        <v>2097152</v>
+      </c>
+      <c r="I24" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -2652,11 +2799,15 @@
       <c r="G25" s="11">
         <v>1</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="15">
+        <f t="shared" si="0"/>
+        <v>4194304</v>
+      </c>
+      <c r="I25" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -2674,11 +2825,15 @@
         <v>3</v>
       </c>
       <c r="G26" s="11"/>
-      <c r="H26" s="11" t="s">
+      <c r="H26" s="15">
+        <f t="shared" si="0"/>
+        <v>8388608</v>
+      </c>
+      <c r="I26" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -2696,84 +2851,88 @@
         <v>3</v>
       </c>
       <c r="G27" s="11"/>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="15">
+        <f t="shared" si="0"/>
+        <v>16777216</v>
+      </c>
+      <c r="I27" s="11" t="s">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B6:F9 B10:D13 F10:F15 B4:H5 H6:H13">
-    <cfRule type="containsBlanks" dxfId="25" priority="15">
+  <conditionalFormatting sqref="B6:F9 B10:D13 F10:F15 B4:I5 I6:I13">
+    <cfRule type="containsBlanks" dxfId="17" priority="15">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:D15 H14:H15 F14:F15">
-    <cfRule type="containsBlanks" dxfId="24" priority="14">
+  <conditionalFormatting sqref="B14:D15 I14:I15 F14:F15">
+    <cfRule type="containsBlanks" dxfId="16" priority="14">
       <formula>LEN(TRIM(B14))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:H17">
-    <cfRule type="containsBlanks" dxfId="23" priority="13">
+  <conditionalFormatting sqref="B16:I17">
+    <cfRule type="containsBlanks" dxfId="15" priority="13">
       <formula>LEN(TRIM(B16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsBlanks" dxfId="22" priority="12">
+    <cfRule type="containsBlanks" dxfId="14" priority="12">
       <formula>LEN(TRIM(C18))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
-    <cfRule type="containsBlanks" dxfId="21" priority="11">
-      <formula>LEN(TRIM(H18))=0</formula>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="containsBlanks" dxfId="13" priority="11">
+      <formula>LEN(TRIM(I18))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:F20 H19:H20">
-    <cfRule type="containsBlanks" dxfId="20" priority="10">
+  <conditionalFormatting sqref="B19:F20 I19:I20">
+    <cfRule type="containsBlanks" dxfId="12" priority="10">
       <formula>LEN(TRIM(B19))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="containsBlanks" dxfId="19" priority="9">
+    <cfRule type="containsBlanks" dxfId="11" priority="9">
       <formula>LEN(TRIM(C21))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="containsBlanks" dxfId="18" priority="8">
-      <formula>LEN(TRIM(H21))=0</formula>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="containsBlanks" dxfId="10" priority="8">
+      <formula>LEN(TRIM(I21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="containsBlanks" dxfId="17" priority="7">
+    <cfRule type="containsBlanks" dxfId="9" priority="7">
       <formula>LEN(TRIM(C22))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22:H27">
-    <cfRule type="containsBlanks" dxfId="16" priority="6">
-      <formula>LEN(TRIM(H22))=0</formula>
+  <conditionalFormatting sqref="I22:I27">
+    <cfRule type="containsBlanks" dxfId="8" priority="6">
+      <formula>LEN(TRIM(I22))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G15">
-    <cfRule type="containsBlanks" dxfId="15" priority="5">
+  <conditionalFormatting sqref="G6:H15">
+    <cfRule type="containsBlanks" dxfId="7" priority="5">
       <formula>LEN(TRIM(G6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:E15">
-    <cfRule type="containsBlanks" dxfId="14" priority="4">
+    <cfRule type="containsBlanks" dxfId="6" priority="4">
       <formula>LEN(TRIM(E10))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G19:G20">
-    <cfRule type="containsBlanks" dxfId="13" priority="3">
+  <conditionalFormatting sqref="G19:H20">
+    <cfRule type="containsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(G19))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:E23">
-    <cfRule type="containsBlanks" dxfId="12" priority="2">
+    <cfRule type="containsBlanks" dxfId="4" priority="2">
       <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25:E26">
-    <cfRule type="containsBlanks" dxfId="11" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(E25))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
hardness of dna for scenequest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/PlayerDna.xlsx
+++ b/ConfigData/Xlsx/PlayerDna.xlsx
@@ -24,7 +24,7 @@
     <author>张剑慧</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="131">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -466,6 +466,114 @@
   </si>
   <si>
     <t>~Calculater</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ename</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hot</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cod</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>thk</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lov</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kil</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ged</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>swd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lef</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>frt</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ret</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>anl</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cil</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tim</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pos</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>src</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ord</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sky</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>die</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wat</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1258,68 +1366,13 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="29">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.39997558519241921"/>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -1425,6 +1478,87 @@
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1694,23 +1828,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:I27" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" tableBorderDxfId="24">
-  <autoFilter ref="A3:I27"/>
-  <sortState ref="A4:D4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:J27" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="A3:J27"/>
+  <sortState ref="A4:E4">
     <sortCondition ref="A3:A4"/>
   </sortState>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Id" dataDxfId="23"/>
-    <tableColumn id="2" name="Name" dataDxfId="22"/>
-    <tableColumn id="5" name="Des" dataDxfId="21"/>
-    <tableColumn id="4" name="MutexId" dataDxfId="20"/>
-    <tableColumn id="6" name="X" dataDxfId="19"/>
-    <tableColumn id="7" name="Y" dataDxfId="18"/>
-    <tableColumn id="8" name="LineType" dataDxfId="2"/>
-    <tableColumn id="9" name="~Calculater" dataDxfId="0">
+  <tableColumns count="10">
+    <tableColumn id="1" name="Id" dataDxfId="25"/>
+    <tableColumn id="2" name="Name" dataDxfId="24"/>
+    <tableColumn id="10" name="Ename" dataDxfId="16"/>
+    <tableColumn id="5" name="Des" dataDxfId="23"/>
+    <tableColumn id="4" name="MutexId" dataDxfId="22"/>
+    <tableColumn id="6" name="X" dataDxfId="21"/>
+    <tableColumn id="7" name="Y" dataDxfId="20"/>
+    <tableColumn id="8" name="LineType" dataDxfId="19"/>
+    <tableColumn id="9" name="~Calculater" dataDxfId="18">
       <calculatedColumnFormula>POWER(2,A4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Url" dataDxfId="1"/>
+    <tableColumn id="3" name="Url" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2037,30 +2172,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="5.25" style="4" customWidth="1"/>
-    <col min="3" max="3" width="24.625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="4.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9.75" style="4" customWidth="1"/>
-    <col min="9" max="10" width="9" style="4"/>
-    <col min="11" max="11" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="4"/>
+    <col min="2" max="3" width="5.25" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="4.5" style="4" customWidth="1"/>
+    <col min="8" max="8" width="6" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.75" style="4" customWidth="1"/>
+    <col min="10" max="11" width="9" style="4"/>
+    <col min="12" max="12" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2068,28 +2203,31 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2097,13 +2235,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>37</v>
@@ -2112,13 +2250,16 @@
         <v>37</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -2126,28 +2267,31 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2155,29 +2299,32 @@
         <v>14</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="10">
+      <c r="E4" s="10">
         <v>2</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0</v>
       </c>
       <c r="F4" s="10">
         <v>0</v>
       </c>
       <c r="G4" s="10">
+        <v>0</v>
+      </c>
+      <c r="H4" s="10">
         <v>2</v>
       </c>
-      <c r="H4" s="14">
-        <f t="shared" ref="H4:H27" si="0">POWER(2,A4)</f>
+      <c r="I4" s="14">
+        <f t="shared" ref="I4:I27" si="0">POWER(2,A4)</f>
         <v>2</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2185,29 +2332,32 @@
         <v>15</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="D5" s="10">
-        <v>1</v>
       </c>
       <c r="E5" s="10">
         <v>1</v>
       </c>
       <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10">
         <v>0</v>
       </c>
-      <c r="G5" s="10">
+      <c r="H5" s="10">
         <v>1</v>
       </c>
-      <c r="H5" s="14">
+      <c r="I5" s="14">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2215,29 +2365,32 @@
         <v>16</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="10">
+      <c r="E6" s="10">
         <v>4</v>
       </c>
-      <c r="E6" s="10">
+      <c r="F6" s="10">
         <v>2</v>
       </c>
-      <c r="F6" s="10">
+      <c r="G6" s="10">
         <v>0</v>
       </c>
-      <c r="G6" s="10">
+      <c r="H6" s="10">
         <v>2</v>
       </c>
-      <c r="H6" s="14">
+      <c r="I6" s="14">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="J6" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2245,29 +2398,32 @@
         <v>73</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="D7" s="10">
-        <v>3</v>
       </c>
       <c r="E7" s="10">
         <v>3</v>
       </c>
       <c r="F7" s="10">
+        <v>3</v>
+      </c>
+      <c r="G7" s="10">
         <v>0</v>
       </c>
-      <c r="G7" s="10">
+      <c r="H7" s="10">
         <v>1</v>
       </c>
-      <c r="H7" s="14">
+      <c r="I7" s="14">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="J7" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2275,29 +2431,32 @@
         <v>17</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="10">
+      <c r="E8" s="10">
         <v>6</v>
       </c>
-      <c r="E8" s="10">
+      <c r="F8" s="10">
         <v>4</v>
       </c>
-      <c r="F8" s="10">
+      <c r="G8" s="10">
         <v>0</v>
       </c>
-      <c r="G8" s="10">
+      <c r="H8" s="10">
         <v>2</v>
       </c>
-      <c r="H8" s="14">
+      <c r="I8" s="14">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2305,29 +2464,32 @@
         <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="D9" s="10">
-        <v>5</v>
       </c>
       <c r="E9" s="10">
         <v>5</v>
       </c>
       <c r="F9" s="10">
+        <v>5</v>
+      </c>
+      <c r="G9" s="10">
         <v>0</v>
       </c>
-      <c r="G9" s="10">
+      <c r="H9" s="10">
         <v>1</v>
       </c>
-      <c r="H9" s="14">
+      <c r="I9" s="14">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="J9" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -2335,29 +2497,32 @@
         <v>65</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="10">
+      <c r="E10" s="10">
         <v>8</v>
       </c>
-      <c r="E10" s="10">
+      <c r="F10" s="10">
         <v>0</v>
       </c>
-      <c r="F10" s="10">
+      <c r="G10" s="10">
         <v>1</v>
       </c>
-      <c r="G10" s="10">
+      <c r="H10" s="10">
         <v>2</v>
       </c>
-      <c r="H10" s="14">
+      <c r="I10" s="14">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="J10" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2365,13 +2530,13 @@
         <v>66</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="10">
+      <c r="E11" s="10">
         <v>7</v>
-      </c>
-      <c r="E11" s="10">
-        <v>1</v>
       </c>
       <c r="F11" s="10">
         <v>1</v>
@@ -2379,15 +2544,18 @@
       <c r="G11" s="10">
         <v>1</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+      <c r="I11" s="14">
         <f t="shared" si="0"/>
         <v>256</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="J11" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2395,29 +2563,32 @@
         <v>51</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="10">
+      <c r="E12" s="10">
         <v>10</v>
       </c>
-      <c r="E12" s="10">
+      <c r="F12" s="10">
         <v>2</v>
       </c>
-      <c r="F12" s="10">
+      <c r="G12" s="10">
         <v>1</v>
       </c>
-      <c r="G12" s="10">
+      <c r="H12" s="10">
         <v>2</v>
       </c>
-      <c r="H12" s="14">
+      <c r="I12" s="14">
         <f t="shared" si="0"/>
         <v>512</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="J12" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2425,29 +2596,32 @@
         <v>52</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="10">
+      <c r="E13" s="10">
         <v>9</v>
       </c>
-      <c r="E13" s="10">
+      <c r="F13" s="10">
         <v>3</v>
-      </c>
-      <c r="F13" s="10">
-        <v>1</v>
       </c>
       <c r="G13" s="10">
         <v>1</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="10">
+        <v>1</v>
+      </c>
+      <c r="I13" s="14">
         <f t="shared" si="0"/>
         <v>1024</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="J13" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -2455,29 +2629,32 @@
         <v>55</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="10">
+      <c r="E14" s="10">
         <v>12</v>
       </c>
-      <c r="E14" s="10">
+      <c r="F14" s="10">
         <v>4</v>
       </c>
-      <c r="F14" s="10">
+      <c r="G14" s="10">
         <v>1</v>
       </c>
-      <c r="G14" s="10">
+      <c r="H14" s="10">
         <v>2</v>
       </c>
-      <c r="H14" s="14">
+      <c r="I14" s="14">
         <f t="shared" si="0"/>
         <v>2048</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="J14" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -2485,455 +2662,424 @@
         <v>56</v>
       </c>
       <c r="C15" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="10">
+      <c r="E15" s="10">
         <v>11</v>
       </c>
-      <c r="E15" s="10">
+      <c r="F15" s="10">
         <v>5</v>
-      </c>
-      <c r="F15" s="10">
-        <v>1</v>
       </c>
       <c r="G15" s="10">
         <v>1</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="10">
+        <v>1</v>
+      </c>
+      <c r="I15" s="14">
         <f t="shared" si="0"/>
         <v>4096</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="J15" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="9">
         <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="10">
+      <c r="F16" s="10">
         <v>0</v>
-      </c>
-      <c r="F16" s="10">
-        <v>2</v>
       </c>
       <c r="G16" s="10">
         <v>2</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="10">
+        <v>2</v>
+      </c>
+      <c r="I16" s="14">
         <f t="shared" si="0"/>
         <v>8192</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="J16" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="9">
         <v>14</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="10">
+      <c r="F17" s="10">
         <v>1</v>
       </c>
-      <c r="F17" s="10">
+      <c r="G17" s="10">
         <v>2</v>
       </c>
-      <c r="G17" s="10">
+      <c r="H17" s="10">
         <v>3</v>
       </c>
-      <c r="H17" s="14">
+      <c r="I17" s="14">
         <f t="shared" si="0"/>
         <v>16384</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="J17" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="9">
         <v>15</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="E18" s="10">
-        <v>2</v>
       </c>
       <c r="F18" s="10">
         <v>2</v>
       </c>
       <c r="G18" s="10">
+        <v>2</v>
+      </c>
+      <c r="H18" s="10">
         <v>1</v>
       </c>
-      <c r="H18" s="14">
+      <c r="I18" s="14">
         <f t="shared" si="0"/>
         <v>32768</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="J18" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="9">
         <v>16</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="10">
+      <c r="F19" s="10">
         <v>3</v>
-      </c>
-      <c r="F19" s="10">
-        <v>2</v>
       </c>
       <c r="G19" s="10">
         <v>2</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="10">
+        <v>2</v>
+      </c>
+      <c r="I19" s="14">
         <f t="shared" si="0"/>
         <v>65536</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="J19" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="9">
         <v>17</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="11">
+      <c r="F20" s="11">
         <v>4</v>
       </c>
-      <c r="F20" s="11">
+      <c r="G20" s="11">
         <v>2</v>
       </c>
-      <c r="G20" s="10">
+      <c r="H20" s="10">
         <v>3</v>
       </c>
-      <c r="H20" s="14">
+      <c r="I20" s="14">
         <f t="shared" si="0"/>
         <v>131072</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="J20" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="9">
         <v>18</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="11">
+      <c r="F21" s="11">
         <v>5</v>
       </c>
-      <c r="F21" s="11">
+      <c r="G21" s="11">
         <v>2</v>
       </c>
-      <c r="G21" s="10">
+      <c r="H21" s="10">
         <v>1</v>
       </c>
-      <c r="H21" s="14">
+      <c r="I21" s="14">
         <f t="shared" si="0"/>
         <v>262144</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="J21" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="9">
         <v>19</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="10">
+      <c r="F22" s="10">
         <v>0</v>
       </c>
-      <c r="F22" s="11">
+      <c r="G22" s="11">
         <v>3</v>
       </c>
-      <c r="G22" s="11">
+      <c r="H22" s="11">
         <v>2</v>
       </c>
-      <c r="H22" s="15">
+      <c r="I22" s="15">
         <f t="shared" si="0"/>
         <v>524288</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="J22" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="9">
         <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="E23" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="10">
+      <c r="F23" s="10">
         <v>1</v>
-      </c>
-      <c r="F23" s="11">
-        <v>3</v>
       </c>
       <c r="G23" s="11">
         <v>3</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="11">
+        <v>3</v>
+      </c>
+      <c r="I23" s="15">
         <f t="shared" si="0"/>
         <v>1048576</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="J23" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="9">
         <v>21</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="10">
+      <c r="F24" s="10">
         <v>2</v>
-      </c>
-      <c r="F24" s="11">
-        <v>3</v>
       </c>
       <c r="G24" s="11">
         <v>3</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="11">
+        <v>3</v>
+      </c>
+      <c r="I24" s="15">
         <f t="shared" si="0"/>
         <v>2097152</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="J24" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="9">
         <v>22</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="E25" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="10">
+      <c r="F25" s="10">
         <v>3</v>
       </c>
-      <c r="F25" s="11">
+      <c r="G25" s="11">
         <v>3</v>
       </c>
-      <c r="G25" s="11">
+      <c r="H25" s="11">
         <v>1</v>
       </c>
-      <c r="H25" s="15">
+      <c r="I25" s="15">
         <f t="shared" si="0"/>
         <v>4194304</v>
       </c>
-      <c r="I25" s="11" t="s">
+      <c r="J25" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="9">
         <v>23</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11">
+      <c r="E26" s="11"/>
+      <c r="F26" s="11">
         <v>4</v>
       </c>
-      <c r="F26" s="11">
+      <c r="G26" s="11">
         <v>3</v>
       </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="15">
+      <c r="H26" s="11"/>
+      <c r="I26" s="15">
         <f t="shared" si="0"/>
         <v>8388608</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="J26" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="9">
         <v>24</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11">
+      <c r="E27" s="11"/>
+      <c r="F27" s="11">
         <v>5</v>
       </c>
-      <c r="F27" s="11">
+      <c r="G27" s="11">
         <v>3</v>
       </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="15">
+      <c r="H27" s="11"/>
+      <c r="I27" s="15">
         <f t="shared" si="0"/>
         <v>16777216</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="J27" s="11" t="s">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B6:F9 B10:D13 F10:F15 B4:I5 I6:I13">
-    <cfRule type="containsBlanks" dxfId="17" priority="15">
+  <conditionalFormatting sqref="B4:J27">
+    <cfRule type="containsBlanks" dxfId="15" priority="15">
       <formula>LEN(TRIM(B4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:D15 I14:I15 F14:F15">
-    <cfRule type="containsBlanks" dxfId="16" priority="14">
-      <formula>LEN(TRIM(B14))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:I17">
-    <cfRule type="containsBlanks" dxfId="15" priority="13">
-      <formula>LEN(TRIM(B16))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="containsBlanks" dxfId="14" priority="12">
-      <formula>LEN(TRIM(C18))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="containsBlanks" dxfId="13" priority="11">
-      <formula>LEN(TRIM(I18))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:F20 I19:I20">
-    <cfRule type="containsBlanks" dxfId="12" priority="10">
-      <formula>LEN(TRIM(B19))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="containsBlanks" dxfId="11" priority="9">
-      <formula>LEN(TRIM(C21))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="containsBlanks" dxfId="10" priority="8">
-      <formula>LEN(TRIM(I21))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22:C27">
-    <cfRule type="containsBlanks" dxfId="9" priority="7">
-      <formula>LEN(TRIM(C22))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22:I27">
-    <cfRule type="containsBlanks" dxfId="8" priority="6">
-      <formula>LEN(TRIM(I22))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6:H15">
-    <cfRule type="containsBlanks" dxfId="7" priority="5">
-      <formula>LEN(TRIM(G6))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E15">
-    <cfRule type="containsBlanks" dxfId="6" priority="4">
-      <formula>LEN(TRIM(E10))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G19:H20">
-    <cfRule type="containsBlanks" dxfId="5" priority="3">
-      <formula>LEN(TRIM(G19))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E23">
-    <cfRule type="containsBlanks" dxfId="4" priority="2">
-      <formula>LEN(TRIM(E22))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25:E26">
-    <cfRule type="containsBlanks" dxfId="3" priority="1">
-      <formula>LEN(TRIM(E25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
a new dna plan
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/PlayerDna.xlsx
+++ b/ConfigData/Xlsx/PlayerDna.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="153">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -155,10 +155,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>17,17</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>16,18</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -457,14 +453,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>计算系数</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>~Calculater</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -574,6 +562,106 @@
   </si>
   <si>
     <t>wat</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>归类</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐藏的对话选项</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>增益难度- 战斗难度+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>17,18</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐藏的对话选项-时间</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐藏的对话选项-绕路</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>boss难度++ 宝物概率+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐藏的对话选项-偷袭</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐藏的对话选项-单挑</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>宝物概率- 战斗难度-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱难度+ 宝物概率+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗概率+ 冒险概率+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>增益难度- 游戏概率+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>困难事件概率+++ 角色概率+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗难度- 角色概率-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色难度+ 游戏难度-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冒险概率+ 交易概率+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗难度- 交易概率-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>游戏概率+ 采集概率+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱难度- 采集概率-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>鉴定难度- 冒险概率-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗概率- 冒险难度+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>游戏难度+ 增益概率+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>增益难度+ 卡牌概率+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冒险难度- 增益概率-</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1315,10 +1403,10 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="49" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1366,109 +1454,30 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="14">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1493,53 +1502,8 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1632,6 +1596,25 @@
         <color theme="1"/>
         <name val="宋体"/>
         <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
@@ -1828,24 +1811,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:J27" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:J27" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="A3:J27"/>
   <sortState ref="A4:E4">
     <sortCondition ref="A3:A4"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="Id" dataDxfId="25"/>
-    <tableColumn id="2" name="Name" dataDxfId="24"/>
-    <tableColumn id="10" name="Ename" dataDxfId="16"/>
-    <tableColumn id="5" name="Des" dataDxfId="23"/>
-    <tableColumn id="4" name="MutexId" dataDxfId="22"/>
-    <tableColumn id="6" name="X" dataDxfId="21"/>
-    <tableColumn id="7" name="Y" dataDxfId="20"/>
-    <tableColumn id="8" name="LineType" dataDxfId="19"/>
-    <tableColumn id="9" name="~Calculater" dataDxfId="18">
+    <tableColumn id="1" name="Id" dataDxfId="10"/>
+    <tableColumn id="2" name="Name" dataDxfId="9"/>
+    <tableColumn id="10" name="Ename" dataDxfId="8"/>
+    <tableColumn id="5" name="Des" dataDxfId="7"/>
+    <tableColumn id="4" name="MutexId" dataDxfId="6"/>
+    <tableColumn id="6" name="X" dataDxfId="5"/>
+    <tableColumn id="7" name="Y" dataDxfId="4"/>
+    <tableColumn id="8" name="LineType" dataDxfId="3"/>
+    <tableColumn id="9" name="~Calculater" dataDxfId="0">
       <calculatedColumnFormula>POWER(2,A4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Url" dataDxfId="17"/>
+    <tableColumn id="3" name="Url" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2178,7 +2161,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2189,7 +2172,7 @@
     <col min="5" max="5" width="12.625" style="4" customWidth="1"/>
     <col min="6" max="7" width="4.5" style="4" customWidth="1"/>
     <col min="8" max="8" width="6" style="4" customWidth="1"/>
-    <col min="9" max="9" width="9.75" style="4" customWidth="1"/>
+    <col min="9" max="9" width="23.125" style="4" customWidth="1"/>
     <col min="10" max="11" width="9" style="4"/>
     <col min="12" max="12" width="9.5" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="4"/>
@@ -2203,7 +2186,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>11</v>
@@ -2212,16 +2195,16 @@
         <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>4</v>
@@ -2235,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>12</v>
@@ -2244,16 +2227,16 @@
         <v>9</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>1</v>
@@ -2267,7 +2250,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>13</v>
@@ -2276,16 +2259,16 @@
         <v>10</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>7</v>
@@ -2299,10 +2282,10 @@
         <v>14</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" s="10">
         <v>2</v>
@@ -2316,12 +2299,11 @@
       <c r="H4" s="10">
         <v>2</v>
       </c>
-      <c r="I4" s="14">
-        <f t="shared" ref="I4:I27" si="0">POWER(2,A4)</f>
-        <v>2</v>
+      <c r="I4" s="14" t="s">
+        <v>144</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
@@ -2332,10 +2314,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="10">
         <v>1</v>
@@ -2349,12 +2331,11 @@
       <c r="H5" s="10">
         <v>1</v>
       </c>
-      <c r="I5" s="14">
-        <f t="shared" si="0"/>
-        <v>4</v>
+      <c r="I5" s="14" t="s">
+        <v>142</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
@@ -2365,10 +2346,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="10">
         <v>4</v>
@@ -2382,12 +2363,11 @@
       <c r="H6" s="10">
         <v>2</v>
       </c>
-      <c r="I6" s="14">
-        <f t="shared" si="0"/>
-        <v>8</v>
+      <c r="I6" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
@@ -2395,13 +2375,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" s="10">
         <v>3</v>
@@ -2415,12 +2395,11 @@
       <c r="H7" s="10">
         <v>1</v>
       </c>
-      <c r="I7" s="14">
-        <f t="shared" si="0"/>
-        <v>16</v>
+      <c r="I7" s="14" t="s">
+        <v>148</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
@@ -2431,10 +2410,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" s="10">
         <v>6</v>
@@ -2448,12 +2427,11 @@
       <c r="H8" s="10">
         <v>2</v>
       </c>
-      <c r="I8" s="14">
-        <f t="shared" si="0"/>
-        <v>32</v>
+      <c r="I8" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
@@ -2464,10 +2442,10 @@
         <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9" s="10">
         <v>5</v>
@@ -2481,12 +2459,11 @@
       <c r="H9" s="10">
         <v>1</v>
       </c>
-      <c r="I9" s="14">
-        <f t="shared" si="0"/>
-        <v>64</v>
+      <c r="I9" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
@@ -2494,13 +2471,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E10" s="10">
         <v>8</v>
@@ -2514,12 +2491,11 @@
       <c r="H10" s="10">
         <v>2</v>
       </c>
-      <c r="I10" s="14">
-        <f t="shared" si="0"/>
-        <v>128</v>
+      <c r="I10" s="14" t="s">
+        <v>138</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
@@ -2527,13 +2503,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" s="10">
         <v>7</v>
@@ -2547,12 +2523,11 @@
       <c r="H11" s="10">
         <v>1</v>
       </c>
-      <c r="I11" s="14">
-        <f t="shared" si="0"/>
-        <v>256</v>
+      <c r="I11" s="14" t="s">
+        <v>139</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
@@ -2560,13 +2535,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" s="10">
         <v>10</v>
@@ -2580,12 +2555,11 @@
       <c r="H12" s="10">
         <v>2</v>
       </c>
-      <c r="I12" s="14">
-        <f t="shared" si="0"/>
-        <v>512</v>
+      <c r="I12" s="14" t="s">
+        <v>135</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
@@ -2593,13 +2567,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13" s="10">
         <v>9</v>
@@ -2613,12 +2587,11 @@
       <c r="H13" s="10">
         <v>1</v>
       </c>
-      <c r="I13" s="14">
-        <f t="shared" si="0"/>
-        <v>1024</v>
+      <c r="I13" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
@@ -2626,13 +2599,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E14" s="10">
         <v>12</v>
@@ -2646,12 +2619,11 @@
       <c r="H14" s="10">
         <v>2</v>
       </c>
-      <c r="I14" s="14">
-        <f t="shared" si="0"/>
-        <v>2048</v>
+      <c r="I14" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
@@ -2659,13 +2631,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E15" s="10">
         <v>11</v>
@@ -2679,12 +2651,11 @@
       <c r="H15" s="10">
         <v>1</v>
       </c>
-      <c r="I15" s="14">
-        <f t="shared" si="0"/>
-        <v>4096</v>
+      <c r="I15" s="14" t="s">
+        <v>130</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
@@ -2692,13 +2663,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>19</v>
@@ -2712,12 +2683,11 @@
       <c r="H16" s="10">
         <v>2</v>
       </c>
-      <c r="I16" s="14">
-        <f t="shared" si="0"/>
-        <v>8192</v>
+      <c r="I16" s="14" t="s">
+        <v>149</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
@@ -2725,13 +2695,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>21</v>
@@ -2745,12 +2715,11 @@
       <c r="H17" s="10">
         <v>3</v>
       </c>
-      <c r="I17" s="14">
-        <f t="shared" si="0"/>
-        <v>16384</v>
+      <c r="I17" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
@@ -2758,13 +2727,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>20</v>
@@ -2778,12 +2747,11 @@
       <c r="H18" s="10">
         <v>1</v>
       </c>
-      <c r="I18" s="14">
-        <f t="shared" si="0"/>
-        <v>32768</v>
+      <c r="I18" s="14" t="s">
+        <v>140</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
@@ -2794,13 +2762,13 @@
         <v>22</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>25</v>
+        <v>131</v>
       </c>
       <c r="F19" s="10">
         <v>3</v>
@@ -2811,12 +2779,11 @@
       <c r="H19" s="10">
         <v>2</v>
       </c>
-      <c r="I19" s="14">
-        <f t="shared" si="0"/>
-        <v>65536</v>
+      <c r="I19" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
@@ -2827,13 +2794,13 @@
         <v>23</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" s="11">
         <v>4</v>
@@ -2844,12 +2811,11 @@
       <c r="H20" s="10">
         <v>3</v>
       </c>
-      <c r="I20" s="14">
-        <f t="shared" si="0"/>
-        <v>131072</v>
+      <c r="I20" s="14" t="s">
+        <v>133</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
@@ -2860,13 +2826,13 @@
         <v>24</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F21" s="11">
         <v>5</v>
@@ -2877,12 +2843,11 @@
       <c r="H21" s="10">
         <v>1</v>
       </c>
-      <c r="I21" s="14">
-        <f t="shared" si="0"/>
-        <v>262144</v>
+      <c r="I21" s="14" t="s">
+        <v>152</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
@@ -2890,16 +2855,16 @@
         <v>19</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22" s="10">
         <v>0</v>
@@ -2910,12 +2875,11 @@
       <c r="H22" s="11">
         <v>2</v>
       </c>
-      <c r="I22" s="15">
-        <f t="shared" si="0"/>
-        <v>524288</v>
+      <c r="I22" s="15" t="s">
+        <v>137</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
@@ -2923,16 +2887,16 @@
         <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F23" s="10">
         <v>1</v>
@@ -2943,12 +2907,11 @@
       <c r="H23" s="11">
         <v>3</v>
       </c>
-      <c r="I23" s="15">
-        <f t="shared" si="0"/>
-        <v>1048576</v>
+      <c r="I23" s="15" t="s">
+        <v>151</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
@@ -2956,16 +2919,16 @@
         <v>21</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F24" s="10">
         <v>2</v>
@@ -2976,12 +2939,11 @@
       <c r="H24" s="11">
         <v>3</v>
       </c>
-      <c r="I24" s="15">
-        <f t="shared" si="0"/>
-        <v>2097152</v>
+      <c r="I24" s="15" t="s">
+        <v>139</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
@@ -2989,16 +2951,16 @@
         <v>22</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25" s="10">
         <v>3</v>
@@ -3009,12 +2971,11 @@
       <c r="H25" s="11">
         <v>1</v>
       </c>
-      <c r="I25" s="15">
-        <f t="shared" si="0"/>
-        <v>4194304</v>
+      <c r="I25" s="15" t="s">
+        <v>143</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.15">
@@ -3022,13 +2983,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="11">
@@ -3038,12 +2999,11 @@
         <v>3</v>
       </c>
       <c r="H26" s="11"/>
-      <c r="I26" s="15">
-        <f t="shared" si="0"/>
-        <v>8388608</v>
+      <c r="I26" s="15" t="s">
+        <v>134</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
@@ -3051,13 +3011,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11">
@@ -3067,18 +3027,17 @@
         <v>3</v>
       </c>
       <c r="H27" s="11"/>
-      <c r="I27" s="15">
-        <f t="shared" si="0"/>
-        <v>16777216</v>
+      <c r="I27" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B4:J27">
-    <cfRule type="containsBlanks" dxfId="15" priority="15">
+    <cfRule type="containsBlanks" dxfId="1" priority="15">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
identify the dna icon name
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/PlayerDna.xlsx
+++ b/ConfigData/Xlsx/PlayerDna.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="131">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -215,41 +215,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ice</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fire</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>slow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fast</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ghost</t>
-  </si>
-  <si>
-    <t>kill</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ba</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>xu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hun</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>sky</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -266,10 +231,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>sword</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>叶</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -278,38 +239,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ye</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>guo</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>kong</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>yuan</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>reng</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>tan</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>nu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>贪</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -318,18 +247,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>fang</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>jiao</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>round</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>方</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -446,10 +363,6 @@
   </si>
   <si>
     <t>【高难度】一泓清水明月照</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hong</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1470,16 +1383,8 @@
         <color theme="1"/>
         <name val="宋体"/>
         <family val="3"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1502,8 +1407,17 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1825,10 +1739,10 @@
     <tableColumn id="6" name="X" dataDxfId="5"/>
     <tableColumn id="7" name="Y" dataDxfId="4"/>
     <tableColumn id="8" name="LineType" dataDxfId="3"/>
-    <tableColumn id="9" name="~Calculater" dataDxfId="0">
+    <tableColumn id="9" name="~Calculater" dataDxfId="2">
       <calculatedColumnFormula>POWER(2,A4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Url" dataDxfId="2"/>
+    <tableColumn id="3" name="Url" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2161,7 +2075,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2186,7 +2100,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>11</v>
@@ -2204,7 +2118,7 @@
         <v>38</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>4</v>
@@ -2218,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>12</v>
@@ -2250,7 +2164,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>13</v>
@@ -2268,7 +2182,7 @@
         <v>39</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>7</v>
@@ -2282,10 +2196,10 @@
         <v>14</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="E4" s="10">
         <v>2</v>
@@ -2300,10 +2214,10 @@
         <v>2</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>41</v>
+        <v>122</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
@@ -2314,10 +2228,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="E5" s="10">
         <v>1</v>
@@ -2332,10 +2246,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>40</v>
+        <v>120</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
@@ -2346,10 +2260,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="E6" s="10">
         <v>4</v>
@@ -2364,10 +2278,10 @@
         <v>2</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>43</v>
+        <v>125</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
@@ -2375,13 +2289,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="E7" s="10">
         <v>3</v>
@@ -2396,10 +2310,10 @@
         <v>1</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>42</v>
+        <v>126</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
@@ -2410,10 +2324,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="E8" s="10">
         <v>6</v>
@@ -2428,10 +2342,10 @@
         <v>2</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>61</v>
+        <v>107</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
@@ -2442,10 +2356,10 @@
         <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="E9" s="10">
         <v>5</v>
@@ -2460,10 +2374,10 @@
         <v>1</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>45</v>
+        <v>123</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
@@ -2471,13 +2385,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="E10" s="10">
         <v>8</v>
@@ -2492,10 +2406,10 @@
         <v>2</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>62</v>
+        <v>116</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
@@ -2503,13 +2417,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="E11" s="10">
         <v>7</v>
@@ -2524,10 +2438,10 @@
         <v>1</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>63</v>
+        <v>117</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
@@ -2535,13 +2449,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E12" s="10">
         <v>10</v>
@@ -2556,10 +2470,10 @@
         <v>2</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>52</v>
+        <v>113</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
@@ -2567,13 +2481,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E13" s="10">
         <v>9</v>
@@ -2588,10 +2502,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>53</v>
+        <v>114</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
@@ -2599,13 +2513,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="E14" s="10">
         <v>12</v>
@@ -2620,10 +2534,10 @@
         <v>2</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>56</v>
+        <v>124</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
@@ -2631,13 +2545,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="E15" s="10">
         <v>11</v>
@@ -2652,10 +2566,10 @@
         <v>1</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>57</v>
+        <v>108</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
@@ -2663,13 +2577,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>19</v>
@@ -2684,10 +2598,10 @@
         <v>2</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>66</v>
+        <v>127</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
@@ -2695,13 +2609,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>91</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>21</v>
@@ -2716,10 +2630,10 @@
         <v>3</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>67</v>
+        <v>128</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
@@ -2727,13 +2641,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>20</v>
@@ -2748,10 +2662,10 @@
         <v>1</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
@@ -2762,13 +2676,13 @@
         <v>22</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="F19" s="10">
         <v>3</v>
@@ -2780,10 +2694,10 @@
         <v>2</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>58</v>
+        <v>110</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
@@ -2794,10 +2708,10 @@
         <v>23</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>25</v>
@@ -2812,10 +2726,10 @@
         <v>3</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>59</v>
+        <v>111</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
@@ -2826,10 +2740,10 @@
         <v>24</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>26</v>
@@ -2844,10 +2758,10 @@
         <v>1</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>60</v>
+        <v>130</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
@@ -2858,10 +2772,10 @@
         <v>27</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>31</v>
@@ -2876,10 +2790,10 @@
         <v>2</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>47</v>
+        <v>115</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
@@ -2890,10 +2804,10 @@
         <v>28</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>32</v>
@@ -2908,10 +2822,10 @@
         <v>3</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>48</v>
+        <v>129</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
@@ -2922,10 +2836,10 @@
         <v>30</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>33</v>
@@ -2940,10 +2854,10 @@
         <v>3</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>49</v>
+        <v>117</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
@@ -2954,10 +2868,10 @@
         <v>29</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>34</v>
@@ -2972,10 +2886,10 @@
         <v>1</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.15">
@@ -2983,13 +2897,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="11">
@@ -3000,10 +2914,10 @@
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="J26" s="11" t="s">
-        <v>46</v>
+        <v>112</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
@@ -3011,13 +2925,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11">
@@ -3028,16 +2942,16 @@
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="J27" s="11" t="s">
-        <v>99</v>
+        <v>119</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B4:J27">
-    <cfRule type="containsBlanks" dxfId="1" priority="15">
+    <cfRule type="containsBlanks" dxfId="1" priority="17">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>